<commit_message>
Updating work from day
</commit_message>
<xml_diff>
--- a/Testing_Outputs/feature_coefficients.xlsx
+++ b/Testing_Outputs/feature_coefficients.xlsx
@@ -458,10 +458,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-3.97776658456015</v>
+        <v>-3.981669182352784</v>
       </c>
       <c r="C2" t="n">
-        <v>3.97776658456015</v>
+        <v>3.981669182352784</v>
       </c>
     </row>
     <row r="3">
@@ -471,10 +471,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-3.969261493599962</v>
+        <v>-3.975124635425136</v>
       </c>
       <c r="C3" t="n">
-        <v>3.969261493599962</v>
+        <v>3.975124635425136</v>
       </c>
     </row>
     <row r="4">
@@ -484,10 +484,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3.76986725750588</v>
+        <v>-3.793082060819917</v>
       </c>
       <c r="C4" t="n">
-        <v>3.76986725750588</v>
+        <v>3.793082060819917</v>
       </c>
     </row>
     <row r="5">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-3.763931756587098</v>
+        <v>-3.764159992540425</v>
       </c>
       <c r="C5" t="n">
-        <v>3.763931756587098</v>
+        <v>3.764159992540425</v>
       </c>
     </row>
     <row r="6">
@@ -510,10 +510,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-3.639017810781491</v>
+        <v>-3.641807361289933</v>
       </c>
       <c r="C6" t="n">
-        <v>3.639017810781491</v>
+        <v>3.641807361289933</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-3.618282848922007</v>
+        <v>-3.639304313118213</v>
       </c>
       <c r="C7" t="n">
-        <v>3.618282848922007</v>
+        <v>3.639304313118213</v>
       </c>
     </row>
     <row r="8">
@@ -536,10 +536,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-3.560989595324209</v>
+        <v>-3.566965301078359</v>
       </c>
       <c r="C8" t="n">
-        <v>3.560989595324209</v>
+        <v>3.566965301078359</v>
       </c>
     </row>
     <row r="9">
@@ -549,88 +549,88 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-3.492417692783448</v>
+        <v>-3.530831466607714</v>
       </c>
       <c r="C9" t="n">
-        <v>3.492417692783448</v>
+        <v>3.530831466607714</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>state_CO</t>
+          <t>state_WI</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-3.449440796540373</v>
+        <v>-3.457990115289038</v>
       </c>
       <c r="C10" t="n">
-        <v>3.449440796540373</v>
+        <v>3.457990115289038</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>state_WV</t>
+          <t>state_CO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-3.437104644131678</v>
+        <v>-3.45592962963688</v>
       </c>
       <c r="C11" t="n">
-        <v>3.437104644131678</v>
+        <v>3.45592962963688</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>state_FL</t>
+          <t>state_WV</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-3.405128859385818</v>
+        <v>-3.453748845948945</v>
       </c>
       <c r="C12" t="n">
-        <v>3.405128859385818</v>
+        <v>3.453748845948945</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>state_SD</t>
+          <t>state_DE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-3.398002127247929</v>
+        <v>-3.409149705835587</v>
       </c>
       <c r="C13" t="n">
-        <v>3.398002127247929</v>
+        <v>3.409149705835587</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>state_DE</t>
+          <t>state_FL</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-3.387530117291487</v>
+        <v>-3.406715139305094</v>
       </c>
       <c r="C14" t="n">
-        <v>3.387530117291487</v>
+        <v>3.406715139305094</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>state_WI</t>
+          <t>state_SD</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-3.375950258284826</v>
+        <v>-3.403118777251317</v>
       </c>
       <c r="C15" t="n">
-        <v>3.375950258284826</v>
+        <v>3.403118777251317</v>
       </c>
     </row>
     <row r="16">
@@ -640,10 +640,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-3.373479257497685</v>
+        <v>-3.391842185375438</v>
       </c>
       <c r="C16" t="n">
-        <v>3.373479257497685</v>
+        <v>3.391842185375438</v>
       </c>
     </row>
     <row r="17">
@@ -653,10 +653,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-3.352513087446244</v>
+        <v>-3.370754750738382</v>
       </c>
       <c r="C17" t="n">
-        <v>3.352513087446244</v>
+        <v>3.370754750738382</v>
       </c>
     </row>
     <row r="18">
@@ -666,62 +666,62 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-3.347980769195461</v>
+        <v>-3.36306452122146</v>
       </c>
       <c r="C18" t="n">
-        <v>3.347980769195461</v>
+        <v>3.36306452122146</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>state_CT</t>
+          <t>state_UT</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-3.289450059766077</v>
+        <v>-3.292851006993222</v>
       </c>
       <c r="C19" t="n">
-        <v>3.289450059766077</v>
+        <v>3.292851006993222</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>state_NE</t>
+          <t>state_CT</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-3.281063340018913</v>
+        <v>-3.291100865369797</v>
       </c>
       <c r="C20" t="n">
-        <v>3.281063340018913</v>
+        <v>3.291100865369797</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>state_UT</t>
+          <t>state_NE</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-3.25636008255829</v>
+        <v>-3.276643914791241</v>
       </c>
       <c r="C21" t="n">
-        <v>3.25636008255829</v>
+        <v>3.276643914791241</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>state_OK</t>
+          <t>state_IA</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-3.248318934523048</v>
+        <v>-3.261448502323486</v>
       </c>
       <c r="C22" t="n">
-        <v>3.248318934523048</v>
+        <v>3.261448502323486</v>
       </c>
     </row>
     <row r="23">
@@ -731,257 +731,257 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-3.244962199313525</v>
+        <v>-3.257939412018935</v>
       </c>
       <c r="C23" t="n">
-        <v>3.244962199313525</v>
+        <v>3.257939412018935</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>state_OH</t>
+          <t>state_OR</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-3.227802982904671</v>
+        <v>-3.210176075093548</v>
       </c>
       <c r="C24" t="n">
-        <v>3.227802982904671</v>
+        <v>3.210176075093548</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>state_IA</t>
+          <t>state_NM</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-3.227512084073829</v>
+        <v>-3.206216109984048</v>
       </c>
       <c r="C25" t="n">
-        <v>3.227512084073829</v>
+        <v>3.206216109984048</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>state_IN</t>
+          <t>state_DC</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-3.173611028430942</v>
+        <v>-3.176511644663877</v>
       </c>
       <c r="C26" t="n">
-        <v>3.173611028430942</v>
+        <v>3.176511644663877</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>state_NC</t>
+          <t>state_OH</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-3.163045144500181</v>
+        <v>-3.173047955706903</v>
       </c>
       <c r="C27" t="n">
-        <v>3.163045144500181</v>
+        <v>3.173047955706903</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>state_DC</t>
+          <t>state_OK</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-3.162391495993095</v>
+        <v>-3.157969320596528</v>
       </c>
       <c r="C28" t="n">
-        <v>3.162391495993095</v>
+        <v>3.157969320596528</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>state_WY</t>
+          <t>state_NC</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-3.153485638138096</v>
+        <v>-3.14780411491077</v>
       </c>
       <c r="C29" t="n">
-        <v>3.153485638138096</v>
+        <v>3.14780411491077</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>state_OR</t>
+          <t>state_IN</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-3.152642658346375</v>
+        <v>-3.117028960201333</v>
       </c>
       <c r="C30" t="n">
-        <v>3.152642658346375</v>
+        <v>3.117028960201333</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>state_NM</t>
+          <t>state_KY</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-3.127243872557182</v>
+        <v>-3.108094247739332</v>
       </c>
       <c r="C31" t="n">
-        <v>3.127243872557182</v>
+        <v>3.108094247739332</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>state_NY</t>
+          <t>state_GA</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-3.116994586921533</v>
+        <v>-3.081870491027291</v>
       </c>
       <c r="C32" t="n">
-        <v>3.116994586921533</v>
+        <v>3.081870491027291</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>state_KY</t>
+          <t>state_NY</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-3.088332884887915</v>
+        <v>-3.056178258621492</v>
       </c>
       <c r="C33" t="n">
-        <v>3.088332884887915</v>
+        <v>3.056178258621492</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>state_GA</t>
+          <t>state_MA</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-3.072106306639076</v>
+        <v>-3.046486300793459</v>
       </c>
       <c r="C34" t="n">
-        <v>3.072106306639076</v>
+        <v>3.046486300793459</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>state_MD</t>
+          <t>state_NH</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-3.055761605283015</v>
+        <v>-3.02329792795098</v>
       </c>
       <c r="C35" t="n">
-        <v>3.055761605283015</v>
+        <v>3.02329792795098</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>state_NH</t>
+          <t>state_MI</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-3.00493410501233</v>
+        <v>-3.004660690995528</v>
       </c>
       <c r="C36" t="n">
-        <v>3.00493410501233</v>
+        <v>3.004660690995528</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>state_MI</t>
+          <t>state_KS</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-2.983277566927963</v>
+        <v>-2.937553892513254</v>
       </c>
       <c r="C37" t="n">
-        <v>2.983277566927963</v>
+        <v>2.937553892513254</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>voice mail plan_yes</t>
+          <t>state_WY</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-2.946156352482378</v>
+        <v>-2.931652665211982</v>
       </c>
       <c r="C38" t="n">
-        <v>2.946156352482378</v>
+        <v>2.931652665211982</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>state_KS</t>
+          <t>state_MN</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-2.933126654475189</v>
+        <v>-2.930806808267355</v>
       </c>
       <c r="C39" t="n">
-        <v>2.933126654475189</v>
+        <v>2.930806808267355</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>state_MN</t>
+          <t>state_WA</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-2.902986909825001</v>
+        <v>-2.889301090148507</v>
       </c>
       <c r="C40" t="n">
-        <v>2.902986909825001</v>
+        <v>2.889301090148507</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>state_MA</t>
+          <t>state_MD</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-2.843443631666859</v>
+        <v>-2.887842275003738</v>
       </c>
       <c r="C41" t="n">
-        <v>2.843443631666859</v>
+        <v>2.887842275003738</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>state_WA</t>
+          <t>state_ME</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-2.841963654201038</v>
+        <v>-2.846175120342098</v>
       </c>
       <c r="C42" t="n">
-        <v>2.841963654201038</v>
+        <v>2.846175120342098</v>
       </c>
     </row>
     <row r="43">
@@ -991,88 +991,88 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-2.832162190462595</v>
+        <v>-2.844050006536865</v>
       </c>
       <c r="C43" t="n">
-        <v>2.832162190462595</v>
+        <v>2.844050006536865</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>state_ME</t>
+          <t>state_MS</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-2.782046381177298</v>
+        <v>-2.778472880630927</v>
       </c>
       <c r="C44" t="n">
-        <v>2.782046381177298</v>
+        <v>2.778472880630927</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>state_NV</t>
+          <t>voice mail plan_yes</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-2.709046508038483</v>
+        <v>-2.75948152536455</v>
       </c>
       <c r="C45" t="n">
-        <v>2.709046508038483</v>
+        <v>2.75948152536455</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>state_MS</t>
+          <t>state_NJ</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-2.648476765590552</v>
+        <v>-2.714675733442863</v>
       </c>
       <c r="C46" t="n">
-        <v>2.648476765590552</v>
+        <v>2.714675733442863</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>state_NJ</t>
+          <t>state_PA</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-2.629644240974747</v>
+        <v>-2.708075276360503</v>
       </c>
       <c r="C47" t="n">
-        <v>2.629644240974747</v>
+        <v>2.708075276360503</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>state_PA</t>
+          <t>state_MT</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-2.618550201778169</v>
+        <v>-2.632247547546313</v>
       </c>
       <c r="C48" t="n">
-        <v>2.618550201778169</v>
+        <v>2.632247547546313</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>state_MT</t>
+          <t>state_NV</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>-2.588238333635392</v>
+        <v>-2.59750362405589</v>
       </c>
       <c r="C49" t="n">
-        <v>2.588238333635392</v>
+        <v>2.59750362405589</v>
       </c>
     </row>
     <row r="50">
@@ -1082,10 +1082,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-2.416672190352188</v>
+        <v>-2.473685564763608</v>
       </c>
       <c r="C50" t="n">
-        <v>2.416672190352188</v>
+        <v>2.473685564763608</v>
       </c>
     </row>
     <row r="51">
@@ -1095,10 +1095,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-2.415683936645322</v>
+        <v>-2.441187617920324</v>
       </c>
       <c r="C51" t="n">
-        <v>2.415683936645322</v>
+        <v>2.441187617920324</v>
       </c>
     </row>
     <row r="52">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-2.332305130448096</v>
+        <v>-2.299415234279512</v>
       </c>
       <c r="C52" t="n">
-        <v>2.332305130448096</v>
+        <v>2.299415234279512</v>
       </c>
     </row>
     <row r="53">
@@ -1121,10 +1121,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1.51703860886911</v>
+        <v>1.48370204701723</v>
       </c>
       <c r="C53" t="n">
-        <v>1.51703860886911</v>
+        <v>1.48370204701723</v>
       </c>
     </row>
     <row r="54">
@@ -1134,10 +1134,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.3916476680557941</v>
+        <v>0.3806829395830256</v>
       </c>
       <c r="C54" t="n">
-        <v>0.3916476680557941</v>
+        <v>0.3806829395830256</v>
       </c>
     </row>
     <row r="55">
@@ -1147,192 +1147,192 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.1446154093625406</v>
+        <v>-0.1281835980426144</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1446154093625406</v>
+        <v>0.1281835980426144</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>total intl charge</t>
+          <t>total intl minutes</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.07066259214403933</v>
+        <v>0.06238189539588748</v>
       </c>
       <c r="C56" t="n">
-        <v>0.07066259214403933</v>
+        <v>0.06238189539588748</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>number vmail messages</t>
+          <t>total intl charge</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.06237236362277362</v>
+        <v>0.05948879551605404</v>
       </c>
       <c r="C57" t="n">
-        <v>0.06237236362277362</v>
+        <v>0.05948879551605404</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>total intl minutes</t>
+          <t>number vmail messages</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0.05826339066047475</v>
+        <v>0.05566512891453215</v>
       </c>
       <c r="C58" t="n">
-        <v>0.05826339066047475</v>
+        <v>0.05566512891453215</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>total night charge</t>
+          <t>total day charge</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.009918163512102699</v>
+        <v>-0.03849432958663385</v>
       </c>
       <c r="C59" t="n">
-        <v>0.009918163512102699</v>
+        <v>0.03849432958663385</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>total day minutes</t>
+          <t>total eve charge</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.008934065958572259</v>
+        <v>-0.01999000590256489</v>
       </c>
       <c r="C60" t="n">
-        <v>0.008934065958572259</v>
+        <v>0.01999000590256489</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>total day charge</t>
+          <t>total day minutes</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.004934332624333435</v>
+        <v>0.01574118740154009</v>
       </c>
       <c r="C61" t="n">
-        <v>0.004934332624333435</v>
+        <v>0.01574118740154009</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>total eve minutes</t>
+          <t>total night charge</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.004877134549084597</v>
+        <v>0.01284344418662861</v>
       </c>
       <c r="C62" t="n">
-        <v>0.004877134549084597</v>
+        <v>0.01284344418662861</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>total night minutes</t>
+          <t>total eve minutes</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.002641924427973345</v>
+        <v>0.006163371637639643</v>
       </c>
       <c r="C63" t="n">
-        <v>0.002641924427973345</v>
+        <v>0.006163371637639643</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>total eve charge</t>
+          <t>total night calls</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.002503104084954062</v>
+        <v>-0.001340168132916265</v>
       </c>
       <c r="C64" t="n">
-        <v>0.002503104084954062</v>
+        <v>0.001340168132916265</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>total night calls</t>
+          <t>area code</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>-0.001745617618501688</v>
+        <v>0.001285651930221503</v>
       </c>
       <c r="C65" t="n">
-        <v>0.001745617618501688</v>
+        <v>0.001285651930221503</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>account length</t>
+          <t>total day calls</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.0008992786950649727</v>
+        <v>-0.001226393687414615</v>
       </c>
       <c r="C66" t="n">
-        <v>0.0008992786950649727</v>
+        <v>0.001226393687414615</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>area code</t>
+          <t>total night minutes</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.0006847776834130952</v>
+        <v>0.001200777841236498</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0006847776834130952</v>
+        <v>0.001200777841236498</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>total day calls</t>
+          <t>total eve calls</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>-0.0002651686125629379</v>
+        <v>-0.0004725746123715288</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0002651686125629379</v>
+        <v>0.0004725746123715288</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>total eve calls</t>
+          <t>account length</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.0002462871648606535</v>
+        <v>0.0003565100666003314</v>
       </c>
       <c r="C69" t="n">
-        <v>0.0002462871648606535</v>
+        <v>0.0003565100666003314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>